<commit_message>
this is new project
</commit_message>
<xml_diff>
--- a/MOVIES.xlsx
+++ b/MOVIES.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>MOVIES</t>
   </si>
@@ -57,13 +57,19 @@
     <t>AMARAN</t>
   </si>
   <si>
-    <t>BIOGRAPHY</t>
-  </si>
-  <si>
     <t>KA</t>
   </si>
   <si>
-    <t>CRIME</t>
+    <t>hit 3</t>
+  </si>
+  <si>
+    <t>ROMCOM</t>
+  </si>
+  <si>
+    <t>HORROR</t>
+  </si>
+  <si>
+    <t>BI0</t>
   </si>
 </sst>
 </file>
@@ -106,18 +112,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -417,7 +426,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:L13"/>
+      <selection activeCell="I10" sqref="I10:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -427,435 +436,447 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
         <v>56325</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6">
+      <c r="F4" s="4"/>
+      <c r="G4" s="5">
         <v>45282</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
         <v>8.8000000000000007</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4">
         <v>12305</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="6">
+      <c r="F6" s="4"/>
+      <c r="G6" s="5">
         <v>45728</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
         <v>9.3000000000000007</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>3</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
         <v>28890</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="6">
+      <c r="F8" s="4"/>
+      <c r="G8" s="5">
         <v>45563</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="4">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <v>34457</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5">
+        <v>45596</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4">
+        <v>9.4</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="4">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <v>73893</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5">
+        <v>45597</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1">
+      <c r="A14" s="4">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4">
+        <v>45314</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5">
+        <v>46151</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1">
-        <v>34457</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="6">
-        <v>45596</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1">
-        <v>9.4</v>
-      </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1">
-        <v>73893</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="6">
-        <v>45597</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="A12:B13"/>
     <mergeCell ref="C12:D13"/>
     <mergeCell ref="E12:F13"/>
     <mergeCell ref="G12:H13"/>
     <mergeCell ref="I12:J13"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="K4:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="A8:B9"/>
     <mergeCell ref="C8:D9"/>
     <mergeCell ref="E8:F9"/>
@@ -868,15 +889,12 @@
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="G6:H7"/>
     <mergeCell ref="K6:L7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="E4:F5"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="K4:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="A12:B13"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K22:L22"/>
@@ -890,6 +908,17 @@
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="E4:F5"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
@@ -899,16 +928,6 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="I18:J18"/>
     <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
@@ -923,17 +942,15 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
@@ -947,11 +964,15 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>